<commit_message>
change incidence to cases per year instead of month
</commit_message>
<xml_diff>
--- a/InputForCode_Kenya.xlsx
+++ b/InputForCode_Kenya.xlsx
@@ -406,7 +406,12 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -414,9 +419,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -980,39 +982,39 @@
         <v>25</v>
       </c>
       <c r="B2" s="18">
-        <v>0.23981666666666668</v>
+        <v>2.878</v>
       </c>
       <c r="C2" s="18">
-        <v>0.23981666666666668</v>
+        <v>2.878</v>
       </c>
       <c r="D2" s="18">
-        <v>0.36586416666666666</v>
+        <v>4.39</v>
       </c>
       <c r="E2" s="18">
-        <v>0.29612333333333335</v>
+        <v>3.553</v>
       </c>
       <c r="F2" s="18">
-        <v>0.18924083333333333</v>
+        <v>2.271</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.0</v>
+      <c r="B3" s="19">
+        <v>0.26</v>
+      </c>
+      <c r="C3" s="19">
+        <v>0.26</v>
+      </c>
+      <c r="D3" s="19">
+        <v>0.26</v>
+      </c>
+      <c r="E3" s="19">
+        <v>0.26</v>
+      </c>
+      <c r="F3" s="19">
+        <v>0.26</v>
       </c>
     </row>
   </sheetData>
@@ -1195,16 +1197,16 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1456,19 +1458,19 @@
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="21">
         <v>2.3</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="21">
         <v>4.6</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="21">
         <v>1.57</v>
       </c>
-      <c r="E2" s="21">
-        <v>1.0</v>
-      </c>
-      <c r="F2" s="21">
+      <c r="E2" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="22">
         <v>1.0</v>
       </c>
     </row>
@@ -1521,16 +1523,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="23" t="s">

</xml_diff>